<commit_message>
https://jira.aplana.com/browse/SBRFNDFL-2324 Патч БД 2.1
</commit_message>
<xml_diff>
--- a/database/database-2.1.0/templates/data/ndfl/consolidated_rnu_ndfl/v2016/rnu_ndfl_person_all_db.xlsx
+++ b/database/database-2.1.0/templates/data/ndfl/consolidated_rnu_ndfl/v2016/rnu_ndfl_person_all_db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13875"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Заголовок" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
   <si>
     <t>Подразделение</t>
   </si>
@@ -359,6 +359,9 @@
 право на уменьшение налога на
 фиксированные авансовые платежи.
 Код налогового органа, выдавшего уведомление</t>
+  </si>
+  <si>
+    <t>СНИЛС</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -786,10 +789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:V3"/>
+  <dimension ref="B2:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:V3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -814,9 +817,10 @@
     <col min="20" max="20" width="9.7109375" customWidth="1"/>
     <col min="21" max="21" width="9.42578125" customWidth="1"/>
     <col min="22" max="22" width="10.42578125" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22">
+    <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -880,8 +884,11 @@
       <c r="V2" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="W2" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="2:22" ht="31.5">
+    <row r="3" spans="2:23" ht="31.5">
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
@@ -944,6 +951,9 @@
       </c>
       <c r="V3" s="3" t="s">
         <v>45</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>